<commit_message>
added Alll Moduels Using Excel Sheet
Added Test suit 003 to 007 using NAukri Inputs from Excel sheet successfully
</commit_message>
<xml_diff>
--- a/Naukri_Maven/src/resources/excel/Inputs_Naukri.xlsx
+++ b/Naukri_Maven/src/resources/excel/Inputs_Naukri.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>URL</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t xml:space="preserve"> !@#$ "</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -106,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -129,17 +132,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -148,11 +140,24 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -451,7 +456,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -466,73 +471,73 @@
     <col min="10" max="11" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
-        <v>89</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>